<commit_message>
done, ready to demo
</commit_message>
<xml_diff>
--- a/Post Journal.xlsx
+++ b/Post Journal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" activeTab="5"/>
+    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Pembelian Hutang Belum Ditagih" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="54">
   <si>
     <t>Kontrak Pembelian</t>
   </si>
@@ -177,6 +177,12 @@
   <si>
     <t>Hutang Transport Belum ditagih</t>
   </si>
+  <si>
+    <t>Persediaan Cutting Center</t>
+  </si>
+  <si>
+    <t>Biaya Bahan Baku</t>
+  </si>
 </sst>
 </file>
 
@@ -215,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -239,11 +245,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -273,6 +288,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2282,9 +2302,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -2595,313 +2617,277 @@
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="8" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="3"/>
+      <c r="F18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="B19" s="3"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="B20" s="3"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="3"/>
+      <c r="G20" s="3">
+        <f>SUM(G18:G19)</f>
+        <v>1000000000</v>
+      </c>
+      <c r="H20" s="3">
+        <f>SUM(H18:H19)</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="B21" s="3"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" t="s">
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11">
+      <c r="A23" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B23" s="3">
         <v>1000000000</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="3">
-        <f>B19</f>
+      <c r="C23" s="10"/>
+      <c r="D23" s="3">
+        <f>B23</f>
         <v>1000000000</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F23" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="3">
-        <f>D25+D26-D27</f>
+      <c r="G23" s="3">
+        <f>D29+D30-D31</f>
         <v>759500000</v>
       </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B24" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C20" s="10" t="str">
-        <f t="shared" ref="C20:C21" si="5">C3</f>
+      <c r="C24" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D20" s="3">
-        <f>D19*B20/100</f>
+      <c r="D24" s="3">
+        <f>D23*B24/100</f>
         <v>110000000</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F24" t="s">
         <v>31</v>
       </c>
-      <c r="G20" s="3">
-        <f>D27</f>
+      <c r="G24" s="3">
+        <f>D31</f>
         <v>17500000</v>
       </c>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A25" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B25" s="5">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C21" s="12" t="str">
-        <f t="shared" si="5"/>
+      <c r="C25" s="12" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D21" s="5">
-        <f>D19*B21/100</f>
+      <c r="D25" s="5">
+        <f>D23*B25/100</f>
         <v>25000000</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F25" t="s">
         <v>32</v>
       </c>
-      <c r="G21" s="3">
-        <f>D22</f>
+      <c r="G25" s="3">
+        <f>D26</f>
         <v>300000000</v>
       </c>
-      <c r="H21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B26" s="3">
         <v>300000000</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="3">
-        <f>B22</f>
+      <c r="C26" s="10"/>
+      <c r="D26" s="3">
+        <f>B26</f>
         <v>300000000</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F26" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3">
-        <f>D19</f>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3">
+        <f>D23</f>
         <v>1000000000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" t="s">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B27" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C23" s="10" t="str">
-        <f t="shared" ref="C23:C24" si="6">C3</f>
+      <c r="C27" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D23" s="3">
-        <f>D22*B23/100</f>
+      <c r="D27" s="3">
+        <f>D26*B27/100</f>
         <v>33000000</v>
       </c>
-      <c r="F23" s="11" t="s">
+      <c r="F27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5">
-        <f>D26</f>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5">
+        <f>D30</f>
         <v>77000000</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B28" s="5">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C24" s="12" t="str">
-        <f t="shared" si="6"/>
+      <c r="C28" s="12" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D24" s="5">
-        <f>D22*B24/100</f>
+      <c r="D28" s="5">
+        <f>D26*B28/100</f>
         <v>7500000</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="3">
-        <f t="shared" ref="G24:H24" si="7">SUM(G19:G23)</f>
+      <c r="F28" s="13"/>
+      <c r="G28" s="3">
+        <f t="shared" ref="G28:H28" si="5">SUM(G23:G27)</f>
         <v>1077000000</v>
       </c>
-      <c r="H24" s="3">
-        <f t="shared" si="7"/>
+      <c r="H28" s="3">
+        <f t="shared" si="5"/>
         <v>1077000000</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" t="s">
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B29" s="3">
         <v>700000000</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="3">
-        <f>B25</f>
+      <c r="C29" s="10"/>
+      <c r="D29" s="3">
+        <f>B29</f>
         <v>700000000</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" t="s">
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B30" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C26" s="10" t="str">
-        <f t="shared" ref="C26:C27" si="8">C3</f>
+      <c r="C30" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D26" s="3">
-        <f>D25*B26/100</f>
+      <c r="D30" s="3">
+        <f>D29*B30/100</f>
         <v>77000000</v>
       </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" t="s">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A31" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B31" s="3">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C27" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="C31" s="10" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D27" s="3">
-        <f>D25*B27/100</f>
+      <c r="D31" s="3">
+        <f>D29*B31/100</f>
         <v>17500000</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F31" t="s">
         <v>12</v>
       </c>
-      <c r="G27" s="3">
-        <f t="shared" ref="G27:H27" si="9">G7+G19</f>
+      <c r="G31" s="3">
+        <f t="shared" ref="G31:H31" si="6">G7+G23</f>
         <v>1085000000</v>
       </c>
-      <c r="H27" s="3">
-        <f t="shared" si="9"/>
+      <c r="H31" s="3">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I27" s="3">
-        <f t="shared" ref="I27:I28" si="10">G27-H27</f>
+      <c r="I31" s="3">
+        <f t="shared" ref="I31:I32" si="7">G31-H31</f>
         <v>1085000000</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B28" s="3"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="3"/>
-      <c r="F28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" s="3">
-        <f t="shared" ref="G28:H28" si="11">G8+G20</f>
-        <v>25000000</v>
-      </c>
-      <c r="H28" s="3">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <f t="shared" si="10"/>
-        <v>25000000</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B29" s="3"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="3"/>
-      <c r="F29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="3">
-        <f t="shared" ref="G29:H29" si="12">G9+G21</f>
-        <v>300000000</v>
-      </c>
-      <c r="H29" s="3">
-        <f t="shared" si="12"/>
-        <v>300000000</v>
-      </c>
-      <c r="I29" s="3">
-        <f t="shared" ref="I29:I30" si="13">H29-G29</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B30" s="3"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="3"/>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G30" s="3">
-        <f t="shared" ref="G30:H30" si="14">G10+G23</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="3">
-        <f t="shared" si="14"/>
-        <v>110000000</v>
-      </c>
-      <c r="I30" s="3">
-        <f t="shared" si="13"/>
-        <v>110000000</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B31" s="3"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="3"/>
-      <c r="F31" t="s">
-        <v>35</v>
-      </c>
-      <c r="G31" s="3">
-        <f t="shared" ref="G31:H31" si="15">G14+G22</f>
-        <v>1000000000</v>
-      </c>
-      <c r="H31" s="3">
-        <f t="shared" si="15"/>
-        <v>1000000000</v>
-      </c>
-      <c r="I31" s="3">
-        <f>G31-H31</f>
-        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
@@ -2909,127 +2895,207 @@
       <c r="C32" s="10"/>
       <c r="D32" s="3"/>
       <c r="F32" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G32" s="3">
-        <f t="shared" ref="G32:H32" si="16">G15</f>
+        <f t="shared" ref="G32:H32" si="8">G8+G24</f>
+        <v>25000000</v>
+      </c>
+      <c r="H32" s="3">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="H32" s="3">
-        <f t="shared" si="16"/>
-        <v>1000000000</v>
-      </c>
       <c r="I32" s="3">
-        <f>H32-G32</f>
-        <v>1000000000</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15.75" customHeight="1">
+        <f t="shared" si="7"/>
+        <v>25000000</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="15.75" customHeight="1">
       <c r="B33" s="3"/>
       <c r="C33" s="10"/>
       <c r="D33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-    </row>
-    <row r="34" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="3">
+        <f t="shared" ref="G33:H33" si="9">G9+G25</f>
+        <v>300000000</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="9"/>
+        <v>300000000</v>
+      </c>
+      <c r="I33" s="3">
+        <f t="shared" ref="I33:I34" si="10">H33-G33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" customHeight="1">
       <c r="B34" s="3"/>
       <c r="C34" s="10"/>
       <c r="D34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-    </row>
-    <row r="35" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G34" s="3">
+        <f t="shared" ref="G34:H34" si="11">G10+G27</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="11"/>
+        <v>110000000</v>
+      </c>
+      <c r="I34" s="3">
+        <f t="shared" si="10"/>
+        <v>110000000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="15.75" customHeight="1">
       <c r="B35" s="3"/>
       <c r="C35" s="10"/>
       <c r="D35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F35" t="s">
+        <v>35</v>
+      </c>
+      <c r="G35" s="3">
+        <f t="shared" ref="G35:H35" si="12">G14+G26</f>
+        <v>1000000000</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="12"/>
+        <v>1000000000</v>
+      </c>
+      <c r="I35" s="3">
+        <f>G35-H35</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" customHeight="1">
       <c r="B36" s="3"/>
       <c r="C36" s="10"/>
       <c r="D36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-    </row>
-    <row r="37" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F36" t="s">
+        <v>36</v>
+      </c>
+      <c r="G36" s="3">
+        <f t="shared" ref="G36:H36" si="13">G15</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="3">
+        <f t="shared" si="13"/>
+        <v>1000000000</v>
+      </c>
+      <c r="I36" s="3">
+        <f>H36-G36</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="15.75" customHeight="1">
       <c r="B37" s="3"/>
       <c r="C37" s="10"/>
       <c r="D37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-    </row>
-    <row r="38" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F37" t="str">
+        <f>F18</f>
+        <v>Biaya Bahan Baku</v>
+      </c>
+      <c r="G37" s="3">
+        <f>G18</f>
+        <v>1000000000</v>
+      </c>
+      <c r="H37" s="3">
+        <f>H18</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="19">
+        <f>G37-H37</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="15.75" customHeight="1">
       <c r="B38" s="3"/>
       <c r="C38" s="10"/>
       <c r="D38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-    </row>
-    <row r="39" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F38" t="str">
+        <f>F19</f>
+        <v>Persediaan</v>
+      </c>
+      <c r="G38" s="3">
+        <f>G19</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="3">
+        <f>H19</f>
+        <v>1000000000</v>
+      </c>
+      <c r="I38" s="19">
+        <f>G38-H38</f>
+        <v>-1000000000</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="15.75" customHeight="1">
       <c r="B39" s="3"/>
       <c r="C39" s="10"/>
       <c r="D39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
     </row>
-    <row r="40" spans="2:8" ht="15.75" customHeight="1">
+    <row r="40" spans="2:9" ht="15.75" customHeight="1">
       <c r="B40" s="3"/>
       <c r="C40" s="10"/>
       <c r="D40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
     </row>
-    <row r="41" spans="2:8" ht="15.75" customHeight="1">
+    <row r="41" spans="2:9" ht="15.75" customHeight="1">
       <c r="B41" s="3"/>
       <c r="C41" s="10"/>
       <c r="D41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
     </row>
-    <row r="42" spans="2:8" ht="15.75" customHeight="1">
+    <row r="42" spans="2:9" ht="15.75" customHeight="1">
       <c r="B42" s="3"/>
       <c r="C42" s="10"/>
       <c r="D42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
     </row>
-    <row r="43" spans="2:8" ht="15.75" customHeight="1">
+    <row r="43" spans="2:9" ht="15.75" customHeight="1">
       <c r="B43" s="3"/>
       <c r="C43" s="10"/>
       <c r="D43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
     </row>
-    <row r="44" spans="2:8" ht="15.75" customHeight="1">
+    <row r="44" spans="2:9" ht="15.75" customHeight="1">
       <c r="B44" s="3"/>
       <c r="C44" s="10"/>
       <c r="D44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
-    <row r="45" spans="2:8" ht="15.75" customHeight="1">
+    <row r="45" spans="2:9" ht="15.75" customHeight="1">
       <c r="B45" s="3"/>
       <c r="C45" s="10"/>
       <c r="D45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
-    <row r="46" spans="2:8" ht="15.75" customHeight="1">
+    <row r="46" spans="2:9" ht="15.75" customHeight="1">
       <c r="B46" s="3"/>
       <c r="C46" s="10"/>
       <c r="D46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
-    <row r="47" spans="2:8" ht="15.75" customHeight="1">
+    <row r="47" spans="2:9" ht="15.75" customHeight="1">
       <c r="B47" s="3"/>
       <c r="C47" s="10"/>
       <c r="D47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
-    <row r="48" spans="2:8" ht="15.75" customHeight="1">
+    <row r="48" spans="2:9" ht="15.75" customHeight="1">
       <c r="B48" s="3"/>
       <c r="C48" s="10"/>
       <c r="D48" s="3"/>
@@ -3399,6 +3465,34 @@
       <c r="D100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
+    </row>
+    <row r="101" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B101" s="3"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B102" s="3"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B103" s="3"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B104" s="3"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -3408,10 +3502,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3760,292 +3854,291 @@
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A21" s="8" t="s">
+    <row r="21" spans="1:12">
+      <c r="B21" s="3"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="3"/>
+      <c r="F21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1000000000</v>
+      </c>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="B22" s="3"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="3"/>
+      <c r="F22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="B23" s="3"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="3"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21">
+        <f>SUM(G21:G22)</f>
+        <v>1000000000</v>
+      </c>
+      <c r="H23" s="21">
+        <f>SUM(H21:H22)</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="B24" s="3"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A25" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G25" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H25" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A22" t="s">
+    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B26" s="3">
         <f>B17</f>
         <v>1500000000</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="3">
-        <f>B22</f>
+      <c r="C26" s="10"/>
+      <c r="D26" s="3">
+        <f>B26</f>
         <v>1500000000</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F26" t="s">
         <v>35</v>
       </c>
-      <c r="G22" s="3">
-        <f>D25+D28+D29</f>
+      <c r="G26" s="3">
+        <f>D29+D32+D33</f>
         <v>1615500000</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A23" t="s">
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A27" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B27" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C23" s="10" t="str">
-        <f t="shared" ref="C23:C24" si="6">C3</f>
+      <c r="C27" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D23" s="3">
-        <f>D22*B23/100</f>
+      <c r="D27" s="3">
+        <f>D26*B27/100</f>
         <v>165000000</v>
       </c>
-      <c r="F23" t="s">
+      <c r="F27" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="3">
-        <f>D25+D28</f>
+      <c r="H27" s="3">
+        <f>D29+D32</f>
         <v>1500000000</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A24" s="11" t="s">
+    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A28" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B28" s="5">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C24" s="12" t="str">
-        <f t="shared" si="6"/>
+      <c r="C28" s="12" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D24" s="5">
-        <f>D22*B24/100</f>
+      <c r="D28" s="5">
+        <f>D26*B28/100</f>
         <v>37500000</v>
       </c>
-      <c r="F24" s="11" t="s">
+      <c r="F28" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G24" s="11"/>
-      <c r="H24" s="5">
-        <f>D29</f>
+      <c r="G28" s="11"/>
+      <c r="H28" s="5">
+        <f>D33</f>
         <v>115500000</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" t="s">
+    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A29" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B29" s="3">
         <f>B7</f>
         <v>450000000</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="3">
-        <f>B25</f>
+      <c r="C29" s="10"/>
+      <c r="D29" s="3">
+        <f>B29</f>
         <v>450000000</v>
       </c>
-      <c r="G25" s="3">
-        <f t="shared" ref="G25:H25" si="7">SUM(G22:G24)</f>
+      <c r="G29" s="3">
+        <f t="shared" ref="G29:H29" si="6">SUM(G26:G28)</f>
         <v>1615500000</v>
       </c>
-      <c r="H25" s="3">
-        <f t="shared" si="7"/>
+      <c r="H29" s="3">
+        <f t="shared" si="6"/>
         <v>1615500000</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A26" t="s">
+    <row r="30" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A30" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B30" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C26" s="10" t="str">
-        <f t="shared" ref="C26:C27" si="8">C3</f>
+      <c r="C30" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D26" s="3">
-        <f>D25*B26/100</f>
+      <c r="D30" s="3">
+        <f>D29*B30/100</f>
         <v>49500000</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="11" t="s">
+    <row r="31" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A31" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B31" s="5">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C27" s="12" t="str">
-        <f t="shared" si="8"/>
+      <c r="C31" s="12" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D27" s="5">
-        <f>D25*B27/100</f>
+      <c r="D31" s="5">
+        <f>D29*B31/100</f>
         <v>11250000</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F31" t="s">
         <v>32</v>
       </c>
-      <c r="G27" s="3">
-        <f>D25</f>
+      <c r="G31" s="3">
+        <f>D29</f>
         <v>450000000</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" t="s">
+    <row r="32" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="3">
-        <f>B22-B25</f>
+      <c r="B32" s="3">
+        <f>B26-B29</f>
         <v>1050000000</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="3">
-        <f>B28</f>
+      <c r="C32" s="10"/>
+      <c r="D32" s="3">
+        <f>B32</f>
         <v>1050000000</v>
       </c>
-      <c r="F28" s="11" t="s">
+      <c r="F32" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="11"/>
-      <c r="H28" s="5">
-        <f>D25</f>
+      <c r="G32" s="11"/>
+      <c r="H32" s="5">
+        <f>D29</f>
         <v>450000000</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" t="s">
+    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A33" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B33" s="3">
         <f>$B$3</f>
         <v>11</v>
       </c>
-      <c r="C29" s="10" t="str">
-        <f t="shared" ref="C29:C30" si="9">C3</f>
+      <c r="C33" s="10" t="str">
+        <f>C3</f>
         <v>%</v>
       </c>
-      <c r="D29" s="3">
-        <f>D28*B29/100</f>
+      <c r="D33" s="3">
+        <f>D32*B33/100</f>
         <v>115500000</v>
       </c>
-      <c r="G29" s="3">
-        <f t="shared" ref="G29:H29" si="10">SUM(G27:G28)</f>
+      <c r="G33" s="3">
+        <f t="shared" ref="G33:H33" si="7">SUM(G31:G32)</f>
         <v>450000000</v>
       </c>
-      <c r="H29" s="3">
-        <f t="shared" si="10"/>
+      <c r="H33" s="3">
+        <f t="shared" si="7"/>
         <v>450000000</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" t="s">
+    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+      <c r="A34" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B34" s="3">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C30" s="10" t="str">
-        <f t="shared" si="9"/>
+      <c r="C34" s="10" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D30" s="3">
-        <f>D28*B30/100</f>
+      <c r="D34" s="3">
+        <f>D32*B34/100</f>
         <v>26250000</v>
       </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B31" s="3"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="3"/>
-      <c r="F31" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B32" s="3"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="3"/>
-      <c r="F32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="3">
-        <f>D28+D29</f>
-        <v>1165500000</v>
-      </c>
-      <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B33" s="3"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="3"/>
-      <c r="F33" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5">
-        <f>D28+D29</f>
-        <v>1165500000</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B34" s="3"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="3"/>
-      <c r="G34" s="3">
-        <f t="shared" ref="G34:H34" si="11">SUM(G32:G33)</f>
-        <v>1165500000</v>
-      </c>
-      <c r="H34" s="3">
-        <f t="shared" si="11"/>
-        <v>1165500000</v>
-      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1">
       <c r="B35" s="3"/>
       <c r="C35" s="10"/>
       <c r="D35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
+      <c r="F35" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1">
       <c r="B36" s="3"/>
       <c r="C36" s="10"/>
       <c r="D36" s="3"/>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G36" s="3">
-        <f>D30</f>
-        <v>26250000</v>
+        <f>D32+D33</f>
+        <v>1165500000</v>
       </c>
       <c r="H36" s="3"/>
     </row>
@@ -4054,12 +4147,12 @@
       <c r="C37" s="10"/>
       <c r="D37" s="3"/>
       <c r="F37" s="11" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5">
-        <f>D30</f>
-        <v>26250000</v>
+        <f>D32+D33</f>
+        <v>1165500000</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="15.75" customHeight="1">
@@ -4067,12 +4160,12 @@
       <c r="C38" s="10"/>
       <c r="D38" s="3"/>
       <c r="G38" s="3">
-        <f t="shared" ref="G38:H38" si="12">SUM(G36:G37)</f>
-        <v>26250000</v>
+        <f t="shared" ref="G38:H38" si="8">SUM(G36:G37)</f>
+        <v>1165500000</v>
       </c>
       <c r="H38" s="3">
-        <f t="shared" si="12"/>
-        <v>26250000</v>
+        <f t="shared" si="8"/>
+        <v>1165500000</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="15.75" customHeight="1">
@@ -4083,123 +4176,89 @@
       <c r="H39" s="3"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I40" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="3"/>
+      <c r="F40" t="s">
+        <v>31</v>
+      </c>
+      <c r="G40" s="3">
+        <f>D34</f>
+        <v>26250000</v>
+      </c>
+      <c r="H40" s="3"/>
     </row>
     <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="B41" s="3"/>
       <c r="C41" s="10"/>
       <c r="D41" s="3"/>
-      <c r="F41" t="s">
+      <c r="F41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G41" s="3">
-        <f t="shared" ref="G41:H41" si="13">G7+G13+G32+G37</f>
-        <v>1665000000</v>
-      </c>
-      <c r="H41" s="3">
-        <f t="shared" si="13"/>
-        <v>37500000</v>
-      </c>
-      <c r="I41" s="3">
-        <f>G41-H41</f>
-        <v>1627500000</v>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5">
+        <f>D34</f>
+        <v>26250000</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
       <c r="B42" s="3"/>
       <c r="C42" s="10"/>
       <c r="D42" s="3"/>
-      <c r="F42" t="s">
-        <v>32</v>
-      </c>
       <c r="G42" s="3">
-        <f t="shared" ref="G42:H42" si="14">G8+G27</f>
-        <v>450000000</v>
+        <f t="shared" ref="G42:H42" si="9">SUM(G40:G41)</f>
+        <v>26250000</v>
       </c>
       <c r="H42" s="3">
-        <f t="shared" si="14"/>
-        <v>450000000</v>
-      </c>
-      <c r="I42" s="3">
-        <f t="shared" ref="I42:I43" si="15">H42-G42</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>26250000</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
       <c r="B43" s="3"/>
       <c r="C43" s="10"/>
       <c r="D43" s="3"/>
-      <c r="F43" t="s">
-        <v>33</v>
-      </c>
-      <c r="G43" s="3">
-        <f t="shared" ref="G43:H43" si="16">G9+G24</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="3">
-        <f t="shared" si="16"/>
-        <v>165000000</v>
-      </c>
-      <c r="I43" s="3">
-        <f t="shared" si="15"/>
-        <v>165000000</v>
-      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B44" s="3"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="3"/>
-      <c r="F44" t="s">
-        <v>31</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" ref="G44:H44" si="17">G12+G36</f>
-        <v>37500000</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="I44" s="3">
-        <f t="shared" ref="I44:I45" si="18">G44-H44</f>
-        <v>37500000</v>
-      </c>
+      <c r="A44" s="8"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+      <c r="L44" s="8"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="B45" s="3"/>
       <c r="C45" s="10"/>
       <c r="D45" s="3"/>
       <c r="F45" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="G45" s="3">
-        <f t="shared" ref="G45:H45" si="19">G17+G23</f>
-        <v>1500000000</v>
+        <f t="shared" ref="G45:H45" si="10">G7+G13+G36+G41</f>
+        <v>1665000000</v>
       </c>
       <c r="H45" s="3">
-        <f t="shared" si="19"/>
-        <v>1500000000</v>
+        <f t="shared" si="10"/>
+        <v>37500000</v>
       </c>
       <c r="I45" s="3">
-        <f t="shared" si="18"/>
-        <v>0</v>
+        <f>G45-H45</f>
+        <v>1627500000</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15.75" customHeight="1">
@@ -4207,19 +4266,19 @@
       <c r="C46" s="10"/>
       <c r="D46" s="3"/>
       <c r="F46" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" ref="G46:H46" si="20">G18</f>
+        <f t="shared" ref="G46:H46" si="11">G8+G31</f>
+        <v>450000000</v>
+      </c>
+      <c r="H46" s="3">
+        <f t="shared" si="11"/>
+        <v>450000000</v>
+      </c>
+      <c r="I46" s="3">
+        <f t="shared" ref="I46:I47" si="12">H46-G46</f>
         <v>0</v>
-      </c>
-      <c r="H46" s="3">
-        <f t="shared" si="20"/>
-        <v>1500000000</v>
-      </c>
-      <c r="I46" s="3">
-        <f>H46-G46</f>
-        <v>1500000000</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
@@ -4227,134 +4286,212 @@
       <c r="C47" s="10"/>
       <c r="D47" s="3"/>
       <c r="F47" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" ref="G47:H47" si="21">G22+G28+G33</f>
-        <v>1615500000</v>
+        <f t="shared" ref="G47:H47" si="13">G9+G28</f>
+        <v>0</v>
       </c>
       <c r="H47" s="3">
-        <f t="shared" si="21"/>
-        <v>1615500000</v>
+        <f t="shared" si="13"/>
+        <v>165000000</v>
       </c>
       <c r="I47" s="3">
-        <f>G47-H47</f>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>165000000</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
       <c r="B48" s="3"/>
       <c r="C48" s="10"/>
       <c r="D48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-    </row>
-    <row r="49" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="3">
+        <f t="shared" ref="G48:H48" si="14">G12+G40</f>
+        <v>37500000</v>
+      </c>
+      <c r="H48" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <f t="shared" ref="I48:I49" si="15">G48-H48</f>
+        <v>37500000</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="15.75" customHeight="1">
       <c r="B49" s="3"/>
       <c r="C49" s="10"/>
       <c r="D49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-    </row>
-    <row r="50" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" ref="G49:H49" si="16">G17+G27</f>
+        <v>1500000000</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="16"/>
+        <v>1500000000</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="15.75" customHeight="1">
       <c r="B50" s="3"/>
       <c r="C50" s="10"/>
       <c r="D50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-    </row>
-    <row r="51" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F50" t="s">
+        <v>36</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" ref="G50:H50" si="17">G18</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="17"/>
+        <v>1500000000</v>
+      </c>
+      <c r="I50" s="3">
+        <f>H50-G50</f>
+        <v>1500000000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="15.75" customHeight="1">
       <c r="B51" s="3"/>
       <c r="C51" s="10"/>
       <c r="D51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-    </row>
-    <row r="52" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F51" t="s">
+        <v>35</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" ref="G51:H51" si="18">G26+G32+G37</f>
+        <v>1615500000</v>
+      </c>
+      <c r="H51" s="3">
+        <f t="shared" si="18"/>
+        <v>1615500000</v>
+      </c>
+      <c r="I51" s="3">
+        <f>G51-H51</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="15.75" customHeight="1">
       <c r="B52" s="3"/>
       <c r="C52" s="10"/>
       <c r="D52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-    </row>
-    <row r="53" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F52" t="s">
+        <v>53</v>
+      </c>
+      <c r="G52" s="3">
+        <f>G21</f>
+        <v>1000000000</v>
+      </c>
+      <c r="H52" s="3">
+        <f>H21</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="19">
+        <f>G52-H52</f>
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="15.75" customHeight="1">
       <c r="B53" s="3"/>
       <c r="C53" s="10"/>
       <c r="D53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-    </row>
-    <row r="54" spans="2:8" ht="15.75" customHeight="1">
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="3">
+        <f>G22</f>
+        <v>0</v>
+      </c>
+      <c r="H53" s="3">
+        <f>H22</f>
+        <v>1000000000</v>
+      </c>
+      <c r="I53" s="19">
+        <f>G53-H53</f>
+        <v>-1000000000</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="15.75" customHeight="1">
       <c r="B54" s="3"/>
       <c r="C54" s="10"/>
       <c r="D54" s="3"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="2:8" ht="15.75" customHeight="1">
+    <row r="55" spans="2:9" ht="15.75" customHeight="1">
       <c r="B55" s="3"/>
       <c r="C55" s="10"/>
       <c r="D55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="2:8" ht="15.75" customHeight="1">
+    <row r="56" spans="2:9" ht="15.75" customHeight="1">
       <c r="B56" s="3"/>
       <c r="C56" s="10"/>
       <c r="D56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="2:8" ht="15.75" customHeight="1">
+    <row r="57" spans="2:9" ht="15.75" customHeight="1">
       <c r="B57" s="3"/>
       <c r="C57" s="10"/>
       <c r="D57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="2:8" ht="15.75" customHeight="1">
+    <row r="58" spans="2:9" ht="15.75" customHeight="1">
       <c r="B58" s="3"/>
       <c r="C58" s="10"/>
       <c r="D58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
     </row>
-    <row r="59" spans="2:8" ht="15.75" customHeight="1">
+    <row r="59" spans="2:9" ht="15.75" customHeight="1">
       <c r="B59" s="3"/>
       <c r="C59" s="10"/>
       <c r="D59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
     </row>
-    <row r="60" spans="2:8" ht="15.75" customHeight="1">
+    <row r="60" spans="2:9" ht="15.75" customHeight="1">
       <c r="B60" s="3"/>
       <c r="C60" s="10"/>
       <c r="D60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
     </row>
-    <row r="61" spans="2:8" ht="15.75" customHeight="1">
+    <row r="61" spans="2:9" ht="15.75" customHeight="1">
       <c r="B61" s="3"/>
       <c r="C61" s="10"/>
       <c r="D61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
     </row>
-    <row r="62" spans="2:8" ht="15.75" customHeight="1">
+    <row r="62" spans="2:9" ht="15.75" customHeight="1">
       <c r="B62" s="3"/>
       <c r="C62" s="10"/>
       <c r="D62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
     </row>
-    <row r="63" spans="2:8" ht="15.75" customHeight="1">
+    <row r="63" spans="2:9" ht="15.75" customHeight="1">
       <c r="B63" s="3"/>
       <c r="C63" s="10"/>
       <c r="D63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
     </row>
-    <row r="64" spans="2:8" ht="15.75" customHeight="1">
+    <row r="64" spans="2:9" ht="15.75" customHeight="1">
       <c r="B64" s="3"/>
       <c r="C64" s="10"/>
       <c r="D64" s="3"/>
@@ -4612,6 +4749,34 @@
       <c r="D100" s="3"/>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
+    </row>
+    <row r="101" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B101" s="3"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+    </row>
+    <row r="102" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B102" s="3"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+    </row>
+    <row r="103" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B103" s="3"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+    </row>
+    <row r="104" spans="2:8" ht="15.75" customHeight="1">
+      <c r="B104" s="3"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
@@ -4623,7 +4788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -5754,9 +5921,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -6189,137 +6356,115 @@
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="15">
+    <row r="21" spans="1:11">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="3">
+        <f>D17</f>
         <v>100000000</v>
       </c>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
       <c r="C22" s="4"/>
-      <c r="D22" s="3">
-        <f>B22</f>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
+        <f>D17</f>
         <v>100000000</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G22" s="3">
-        <f>D22</f>
-        <v>100000000</v>
-      </c>
-      <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A23" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B23" s="3">
-        <f>$B$3</f>
-        <v>11</v>
-      </c>
-      <c r="C23" s="4" t="str">
-        <f t="shared" ref="C23:C24" si="6">C3</f>
-        <v>%</v>
-      </c>
-      <c r="D23" s="3">
-        <f>D22*B23/100</f>
-        <v>11000000</v>
-      </c>
+    <row r="23" spans="1:11">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="F23" s="3"/>
       <c r="G23" s="3">
-        <f>D31</f>
-        <v>7700000</v>
-      </c>
-      <c r="H23" s="3"/>
+        <f t="shared" ref="G23:H23" si="6">SUM(G21:G22)</f>
+        <v>100000000</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="6"/>
+        <v>100000000</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="5">
-        <f>$B$4</f>
-        <v>2.5</v>
-      </c>
-      <c r="C24" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>%</v>
-      </c>
-      <c r="D24" s="5">
-        <f>D22*B24/100</f>
-        <v>2500000</v>
-      </c>
+    <row r="24" spans="1:11">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5">
-        <f>D22+D31</f>
-        <v>107700000</v>
-      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3">
-        <f t="shared" ref="G25:H25" si="7">SUM(G22:G24)</f>
-        <v>107700000</v>
-      </c>
-      <c r="H25" s="3">
-        <f t="shared" si="7"/>
-        <v>107700000</v>
-      </c>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
+      <c r="A25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="15">
+        <v>100000000</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <f>B26</f>
+        <v>100000000</v>
+      </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G26" s="3">
+        <f>D26</f>
+        <v>100000000</v>
+      </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
@@ -6327,23 +6472,27 @@
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="15">
-        <v>30000000</v>
-      </c>
-      <c r="C27" s="4"/>
+        <v>2</v>
+      </c>
+      <c r="B27" s="3">
+        <f>$B$3</f>
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="str">
+        <f>C3</f>
+        <v>%</v>
+      </c>
       <c r="D27" s="3">
-        <f>B27</f>
-        <v>30000000</v>
+        <f>D26*B27/100</f>
+        <v>11000000</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="G27" s="3">
-        <f>D27</f>
-        <v>30000000</v>
+        <f>D35</f>
+        <v>7700000</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -6351,76 +6500,58 @@
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="3">
-        <f>$B$3</f>
-        <v>11</v>
-      </c>
-      <c r="C28" s="4" t="str">
-        <f t="shared" ref="C28:C29" si="8">C3</f>
+      <c r="A28" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="5">
+        <f>$B$4</f>
+        <v>2.5</v>
+      </c>
+      <c r="C28" s="6" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D28" s="3">
-        <f>D27*B28/100</f>
-        <v>3300000</v>
+      <c r="D28" s="5">
+        <f>D26*B28/100</f>
+        <v>2500000</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="16" t="s">
-        <v>40</v>
+      <c r="F28" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5">
-        <f>D27</f>
-        <v>30000000</v>
+        <f>D26+D35</f>
+        <v>107700000</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A29" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="5">
-        <f>$B$4</f>
-        <v>2.5</v>
-      </c>
-      <c r="C29" s="6" t="str">
-        <f t="shared" si="8"/>
-        <v>%</v>
-      </c>
-      <c r="D29" s="5">
-        <f>D27*B29/100</f>
-        <v>750000</v>
-      </c>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3">
-        <f t="shared" ref="G29:H29" si="9">SUM(G27:G28)</f>
-        <v>30000000</v>
+        <f t="shared" ref="G29:H29" si="7">SUM(G26:G28)</f>
+        <v>107700000</v>
       </c>
       <c r="H29" s="3">
-        <f t="shared" si="9"/>
-        <v>30000000</v>
+        <f t="shared" si="7"/>
+        <v>107700000</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A30" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="15">
-        <v>70000000</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="3">
-        <f>B30</f>
-        <v>70000000</v>
-      </c>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -6431,23 +6562,24 @@
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="3">
-        <f>$B$3</f>
-        <v>11</v>
-      </c>
-      <c r="C31" s="4" t="str">
-        <f t="shared" ref="C31:C32" si="10">C3</f>
-        <v>%</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B31" s="15">
+        <v>30000000</v>
+      </c>
+      <c r="C31" s="4"/>
       <c r="D31" s="3">
-        <f>D30*B31/100</f>
-        <v>7700000</v>
+        <f>B31</f>
+        <v>30000000</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G31" s="3">
+        <f>D31</f>
+        <v>30000000</v>
+      </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
       <c r="J31" s="3"/>
@@ -6455,95 +6587,130 @@
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
       <c r="A32" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B32" s="3">
+        <f>$B$3</f>
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="str">
+        <f>C3</f>
+        <v>%</v>
+      </c>
+      <c r="D32" s="3">
+        <f>D31*B32/100</f>
+        <v>3300000</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5">
+        <f>D31</f>
+        <v>30000000</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A33" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="5">
         <f>$B$4</f>
         <v>2.5</v>
       </c>
-      <c r="C32" s="4" t="str">
-        <f t="shared" si="10"/>
+      <c r="C33" s="6" t="str">
+        <f>C4</f>
         <v>%</v>
       </c>
-      <c r="D32" s="3">
-        <f>D30*B32/100</f>
-        <v>1750000</v>
-      </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="3"/>
+      <c r="D33" s="5">
+        <f>D31*B33/100</f>
+        <v>750000</v>
+      </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="F33" s="3"/>
       <c r="G33" s="3">
-        <f>D30+D31</f>
-        <v>77700000</v>
-      </c>
-      <c r="H33" s="3"/>
+        <f t="shared" ref="G33:H33" si="8">SUM(G31:G32)</f>
+        <v>30000000</v>
+      </c>
+      <c r="H33" s="3">
+        <f t="shared" si="8"/>
+        <v>30000000</v>
+      </c>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
     </row>
     <row r="34" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
+      <c r="A34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="15">
+        <v>70000000</v>
+      </c>
       <c r="C34" s="4"/>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3">
+        <f>B34</f>
+        <v>70000000</v>
+      </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5">
-        <f>D30+D31</f>
-        <v>77700000</v>
-      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
     </row>
     <row r="35" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="3"/>
+      <c r="A35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" s="3">
+        <f>$B$3</f>
+        <v>11</v>
+      </c>
+      <c r="C35" s="4" t="str">
+        <f>C3</f>
+        <v>%</v>
+      </c>
+      <c r="D35" s="3">
+        <f>D34*B35/100</f>
+        <v>7700000</v>
+      </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="3">
-        <f t="shared" ref="G35:H35" si="11">SUM(G33:G34)</f>
-        <v>77700000</v>
-      </c>
-      <c r="H35" s="3">
-        <f t="shared" si="11"/>
-        <v>77700000</v>
-      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="3">
+        <f>$B$4</f>
+        <v>2.5</v>
+      </c>
+      <c r="C36" s="4" t="str">
+        <f>C4</f>
+        <v>%</v>
+      </c>
+      <c r="D36" s="3">
+        <f>D34*B36/100</f>
+        <v>1750000</v>
+      </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="F36" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
     </row>
@@ -6554,11 +6721,11 @@
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="G37" s="3">
-        <f>D32</f>
-        <v>1750000</v>
+        <f>D34+D35</f>
+        <v>77700000</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -6572,12 +6739,12 @@
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G38" s="5"/>
       <c r="H38" s="5">
-        <f>D32</f>
-        <v>1750000</v>
+        <f>D34+D35</f>
+        <v>77700000</v>
       </c>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -6591,12 +6758,12 @@
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
       <c r="G39" s="3">
-        <f t="shared" ref="G39:H39" si="12">SUM(G37:G38)</f>
-        <v>1750000</v>
+        <f t="shared" ref="G39:H39" si="9">SUM(G37:G38)</f>
+        <v>77700000</v>
       </c>
       <c r="H39" s="3">
-        <f t="shared" si="12"/>
-        <v>1750000</v>
+        <f t="shared" si="9"/>
+        <v>77700000</v>
       </c>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -6621,18 +6788,15 @@
       <c r="C41" s="4"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
-      <c r="F41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="F41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="3">
+        <f>D36</f>
+        <v>1750000</v>
+      </c>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
     </row>
@@ -6642,21 +6806,15 @@
       <c r="C42" s="4"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
-      <c r="F42" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G42" s="3">
-        <f t="shared" ref="G42:H42" si="13">G7+G28</f>
-        <v>30000000</v>
-      </c>
-      <c r="H42" s="3">
-        <f t="shared" si="13"/>
-        <v>30000000</v>
-      </c>
-      <c r="I42" s="3">
-        <f t="shared" ref="I42:I45" si="14">G42-H42</f>
-        <v>0</v>
-      </c>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5">
+        <f>D36</f>
+        <v>1750000</v>
+      </c>
+      <c r="I42" s="3"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
     </row>
@@ -6666,21 +6824,16 @@
       <c r="C43" s="4"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="F43" s="3"/>
       <c r="G43" s="3">
-        <f t="shared" ref="G43:H43" si="15">G8+G23</f>
-        <v>11000000</v>
+        <f t="shared" ref="G43:H43" si="10">SUM(G41:G42)</f>
+        <v>1750000</v>
       </c>
       <c r="H43" s="3">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
-      <c r="I43" s="3">
-        <f t="shared" si="14"/>
-        <v>11000000</v>
-      </c>
+        <f t="shared" si="10"/>
+        <v>1750000</v>
+      </c>
+      <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
     </row>
@@ -6690,21 +6843,10 @@
       <c r="C44" s="4"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="3">
-        <f t="shared" ref="G44:H44" si="16">G9+G12+G34+G37</f>
-        <v>2500000</v>
-      </c>
-      <c r="H44" s="3">
-        <f t="shared" si="16"/>
-        <v>111000000</v>
-      </c>
-      <c r="I44" s="3">
-        <f t="shared" si="14"/>
-        <v>-108500000</v>
-      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
     </row>
@@ -6714,20 +6856,17 @@
       <c r="C45" s="4"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="G45" s="3">
-        <f t="shared" ref="G45:H45" si="17">G17</f>
-        <v>100000000</v>
-      </c>
-      <c r="H45" s="3">
-        <f t="shared" si="17"/>
-        <v>0</v>
-      </c>
-      <c r="I45" s="3">
-        <f t="shared" si="14"/>
-        <v>100000000</v>
+      <c r="F45" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
@@ -6738,19 +6877,19 @@
       <c r="C46" s="4"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
-        <v>43</v>
+      <c r="F46" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="G46" s="3">
-        <f t="shared" ref="G46:H46" si="18">G24+G27+G33</f>
-        <v>107700000</v>
+        <f t="shared" ref="G46:H46" si="11">G7+G32</f>
+        <v>30000000</v>
       </c>
       <c r="H46" s="3">
-        <f t="shared" si="18"/>
-        <v>107700000</v>
+        <f t="shared" si="11"/>
+        <v>30000000</v>
       </c>
       <c r="I46" s="3">
-        <f t="shared" ref="I46:I48" si="19">H46-G46</f>
+        <f t="shared" ref="I46:I49" si="12">G46-H46</f>
         <v>0</v>
       </c>
       <c r="J46" s="3"/>
@@ -6763,19 +6902,19 @@
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G47" s="3">
-        <f t="shared" ref="G47:H47" si="20">G13+G38</f>
+        <f t="shared" ref="G47:H47" si="13">G8+G27</f>
+        <v>11000000</v>
+      </c>
+      <c r="H47" s="3">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="H47" s="3">
-        <f t="shared" si="20"/>
-        <v>2500000</v>
-      </c>
       <c r="I47" s="3">
-        <f t="shared" si="19"/>
-        <v>2500000</v>
+        <f t="shared" si="12"/>
+        <v>11000000</v>
       </c>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -6787,19 +6926,19 @@
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3" t="s">
-        <v>50</v>
+        <v>12</v>
       </c>
       <c r="G48" s="3">
-        <f t="shared" ref="G48:H48" si="21">G18+G22</f>
-        <v>100000000</v>
+        <f t="shared" ref="G48:H48" si="14">G9+G12+G38+G41</f>
+        <v>2500000</v>
       </c>
       <c r="H48" s="3">
-        <f t="shared" si="21"/>
-        <v>100000000</v>
+        <f t="shared" si="14"/>
+        <v>111000000</v>
       </c>
       <c r="I48" s="3">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" si="12"/>
+        <v>-108500000</v>
       </c>
       <c r="J48" s="3"/>
       <c r="K48" s="3"/>
@@ -6810,10 +6949,21 @@
       <c r="C49" s="4"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="F49" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" s="3">
+        <f t="shared" ref="G49:H49" si="15">G17</f>
+        <v>100000000</v>
+      </c>
+      <c r="H49" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="I49" s="3">
+        <f t="shared" si="12"/>
+        <v>100000000</v>
+      </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
     </row>
@@ -6823,10 +6973,21 @@
       <c r="C50" s="4"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="F50" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="3">
+        <f t="shared" ref="G50:H50" si="16">G28+G31+G37</f>
+        <v>107700000</v>
+      </c>
+      <c r="H50" s="3">
+        <f t="shared" si="16"/>
+        <v>107700000</v>
+      </c>
+      <c r="I50" s="3">
+        <f t="shared" ref="I50:I52" si="17">H50-G50</f>
+        <v>0</v>
+      </c>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
     </row>
@@ -6836,10 +6997,21 @@
       <c r="C51" s="4"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
+      <c r="F51" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="3">
+        <f t="shared" ref="G51:H51" si="18">G13+G42</f>
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <f t="shared" si="18"/>
+        <v>2500000</v>
+      </c>
+      <c r="I51" s="3">
+        <f t="shared" si="17"/>
+        <v>2500000</v>
+      </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
     </row>
@@ -6849,10 +7021,21 @@
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
+      <c r="F52" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G52" s="3">
+        <f t="shared" ref="G52:H52" si="19">G18+G26</f>
+        <v>100000000</v>
+      </c>
+      <c r="H52" s="3">
+        <f t="shared" si="19"/>
+        <v>100000000</v>
+      </c>
+      <c r="I52" s="3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
     </row>
@@ -6862,10 +7045,21 @@
       <c r="C53" s="4"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" s="3">
+        <f>G21</f>
+        <v>100000000</v>
+      </c>
+      <c r="H53" s="3">
+        <f>H21</f>
+        <v>0</v>
+      </c>
+      <c r="I53" s="3">
+        <f>G53-H53</f>
+        <v>100000000</v>
+      </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
     </row>
@@ -6875,10 +7069,21 @@
       <c r="C54" s="4"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
+      <c r="F54" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54" s="3">
+        <f>G22</f>
+        <v>0</v>
+      </c>
+      <c r="H54" s="3">
+        <f>H22</f>
+        <v>100000000</v>
+      </c>
+      <c r="I54" s="3">
+        <f>G54-H54</f>
+        <v>-100000000</v>
+      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
     </row>
@@ -7480,6 +7685,58 @@
       <c r="J100" s="3"/>
       <c r="K100" s="3"/>
     </row>
+    <row r="101" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A101" s="3"/>
+      <c r="B101" s="3"/>
+      <c r="C101" s="4"/>
+      <c r="D101" s="3"/>
+      <c r="E101" s="3"/>
+      <c r="F101" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
+      <c r="J101" s="3"/>
+      <c r="K101" s="3"/>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A102" s="3"/>
+      <c r="B102" s="3"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+    </row>
+    <row r="103" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="4"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3"/>
+      <c r="H103" s="3"/>
+      <c r="I103" s="3"/>
+      <c r="J103" s="3"/>
+      <c r="K103" s="3"/>
+    </row>
+    <row r="104" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A104" s="3"/>
+      <c r="B104" s="3"/>
+      <c r="C104" s="4"/>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3"/>
+      <c r="G104" s="3"/>
+      <c r="H104" s="3"/>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -7490,8 +7747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -7501,7 +7758,7 @@
     <col min="3" max="3" width="4" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="31" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.7109375" customWidth="1"/>
     <col min="10" max="11" width="8.7109375" customWidth="1"/>

</xml_diff>